<commit_message>
updating prices at 10:11:52
</commit_message>
<xml_diff>
--- a/script/modules/data/resources/constructor_df.xlsx
+++ b/script/modules/data/resources/constructor_df.xlsx
@@ -474,13 +474,13 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>$32.2m
+          <t>$32.3m
     $0.0m</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>218 pts</t>
+          <t>260 pts</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -502,13 +502,13 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>$26.3m
-    $0.2m</t>
+          <t>$26.2m
+    $0.1m</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>63 pts</t>
+          <t>97 pts</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -525,18 +525,18 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>21%</t>
+          <t>20%</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>$24.3m
-    $0.1m</t>
+          <t>$24.2m
+    $0.0m</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>120 pts</t>
+          <t>177 pts</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -564,7 +564,7 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>90 pts</t>
+          <t>108 pts</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -587,12 +587,12 @@
       <c r="C6" t="inlineStr">
         <is>
           <t>$12.6m
-    $0.1m</t>
+    $0.0m</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>47 pts</t>
+          <t>66 pts</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -615,12 +615,12 @@
       <c r="C7" t="inlineStr">
         <is>
           <t>$12.1m
-    $0.1m</t>
+    $0.0m</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>56 pts</t>
+          <t>103 pts</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -637,18 +637,18 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>17%</t>
+          <t>18%</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>$10.8m
-    $0.3m</t>
+          <t>$10.9m
+    $0.1m</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>94 pts</t>
+          <t>101 pts</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -676,7 +676,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>57 pts</t>
+          <t>62 pts</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -699,12 +699,12 @@
       <c r="C10" t="inlineStr">
         <is>
           <t>$7.4m
-    $0.1m</t>
+    $0.0m</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>43 pts</t>
+          <t>48 pts</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -732,7 +732,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>12 pts</t>
+          <t>33 pts</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">

</xml_diff>